<commit_message>
added acknowledge to status
</commit_message>
<xml_diff>
--- a/Protocol.xlsx
+++ b/Protocol.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Desktop\vUSBnRF24\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Documents\GitHub\vUSBnRF24\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="59">
   <si>
     <t>Description</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>flush buffers, reset configuration. no data payload</t>
+  </si>
+  <si>
+    <t>Last TX Acknowledged</t>
   </si>
 </sst>
 </file>
@@ -648,145 +651,145 @@
   </cellStyleXfs>
   <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -882,6 +885,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -917,6 +937,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1069,871 +1106,882 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q40"/>
+  <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" style="25" customWidth="1"/>
-    <col min="2" max="2" width="3.33203125" style="25" customWidth="1"/>
-    <col min="3" max="3" width="6.5546875" style="25" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" style="25" customWidth="1"/>
-    <col min="5" max="5" width="18" style="25" customWidth="1"/>
-    <col min="6" max="6" width="8.21875" style="25" customWidth="1"/>
-    <col min="7" max="7" width="5.88671875" style="25" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" style="25" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" style="25" customWidth="1"/>
-    <col min="10" max="10" width="3.77734375" style="25" customWidth="1"/>
-    <col min="11" max="11" width="5.88671875" style="25" customWidth="1"/>
-    <col min="12" max="12" width="19" style="25" customWidth="1"/>
-    <col min="13" max="13" width="13.109375" style="25" customWidth="1"/>
-    <col min="14" max="14" width="3" style="25" customWidth="1"/>
-    <col min="15" max="16384" width="11.5546875" style="25"/>
+    <col min="1" max="1" width="19.44140625" style="23" customWidth="1"/>
+    <col min="2" max="2" width="3.33203125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" style="23" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" style="23" customWidth="1"/>
+    <col min="5" max="5" width="18" style="23" customWidth="1"/>
+    <col min="6" max="6" width="8.21875" style="23" customWidth="1"/>
+    <col min="7" max="7" width="5.88671875" style="23" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" style="23" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" style="23" customWidth="1"/>
+    <col min="10" max="10" width="3.77734375" style="23" customWidth="1"/>
+    <col min="11" max="11" width="5.88671875" style="23" customWidth="1"/>
+    <col min="12" max="12" width="19" style="23" customWidth="1"/>
+    <col min="13" max="13" width="13.109375" style="23" customWidth="1"/>
+    <col min="14" max="14" width="3" style="23" customWidth="1"/>
+    <col min="15" max="16384" width="11.5546875" style="23"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="24"/>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="24"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="29" t="s">
+      <c r="A3" s="22"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
     </row>
     <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="24"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="3" t="s">
+      <c r="A4" s="22"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="3" t="s">
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="29"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="24"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
     </row>
     <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="24"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="4" t="s">
+      <c r="A5" s="22"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="29"/>
-      <c r="G5" s="4" t="s">
+      <c r="F5" s="27"/>
+      <c r="G5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="29"/>
-      <c r="K5" s="4" t="s">
+      <c r="J5" s="27"/>
+      <c r="K5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="M5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="18"/>
-      <c r="O5" s="24"/>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="24"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6" s="24"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="8" t="s">
+      <c r="A6" s="22"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="29"/>
-      <c r="G6" s="11">
+      <c r="F6" s="27"/>
+      <c r="G6" s="9">
         <v>7</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="12"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="11" t="s">
+      <c r="I6" s="10"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="9" t="s">
+      <c r="L6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="12" t="s">
+      <c r="M6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="18"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="24"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="13">
+      <c r="A7" s="22"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="11">
         <v>10</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="29"/>
-      <c r="G7" s="16">
+      <c r="F7" s="27"/>
+      <c r="G7" s="14">
         <v>6</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="18"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="16" t="s">
+      <c r="I7" s="16"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="17" t="s">
+      <c r="L7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="M7" s="18" t="s">
+      <c r="M7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="N7" s="18"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="24"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
     </row>
     <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="24"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="13">
+      <c r="A8" s="22"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="11">
         <v>11</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="29"/>
-      <c r="G8" s="19" t="s">
+      <c r="F8" s="27"/>
+      <c r="G8" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="29"/>
-      <c r="K8" s="19" t="s">
+      <c r="J8" s="27"/>
+      <c r="K8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L8" s="20" t="s">
+      <c r="L8" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="21"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="24"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22"/>
     </row>
     <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="24"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="22" t="s">
+      <c r="A9" s="22"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
     </row>
     <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="24"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="33"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="24"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22"/>
     </row>
     <row r="11" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="24"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="24"/>
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="22"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="24"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="37"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="35"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="22"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="24"/>
-      <c r="B13" s="38"/>
-      <c r="C13" s="31" t="s">
+      <c r="A13" s="22"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="F13" s="31"/>
-      <c r="G13" s="2" t="s">
+      <c r="F13" s="29"/>
+      <c r="G13" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="39"/>
-      <c r="O13" s="24"/>
-      <c r="P13" s="24"/>
-      <c r="Q13" s="24"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="47"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="22"/>
+      <c r="P13" s="22"/>
+      <c r="Q13" s="22"/>
     </row>
     <row r="14" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="24"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="41"/>
-      <c r="J14" s="41"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="42"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="24"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="22"/>
     </row>
     <row r="15" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="24"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="24"/>
+      <c r="A15" s="22"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="22"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B16" s="35"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="36"/>
-      <c r="N16" s="37"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="35"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B17" s="38"/>
-      <c r="C17" s="31" t="s">
+      <c r="B17" s="36"/>
+      <c r="C17" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="31" t="s">
+      <c r="E17" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="39"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="37"/>
     </row>
     <row r="18" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="38"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="3" t="s">
+      <c r="B18" s="36"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I18" s="29"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="39"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="47"/>
+      <c r="L18" s="47"/>
+      <c r="M18" s="47"/>
+      <c r="N18" s="37"/>
     </row>
     <row r="19" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="38"/>
-      <c r="C19" s="4" t="s">
+      <c r="B19" s="36"/>
+      <c r="C19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="31"/>
-      <c r="G19" s="43" t="s">
+      <c r="F19" s="29"/>
+      <c r="G19" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="H19" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="I19" s="44" t="s">
+      <c r="I19" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="J19" s="31"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="39"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="47"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="47"/>
+      <c r="N19" s="37"/>
     </row>
     <row r="20" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="38"/>
-      <c r="C20" s="43">
+      <c r="B20" s="36"/>
+      <c r="C20" s="41">
         <v>0</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="44" t="s">
+      <c r="E20" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="F20" s="31"/>
-      <c r="G20" s="45" t="s">
+      <c r="F20" s="29"/>
+      <c r="G20" s="9">
+        <v>7</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I20" s="10"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="47"/>
+      <c r="M20" s="47"/>
+      <c r="N20" s="37"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B21" s="36"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="H20" s="46" t="s">
+      <c r="H21" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="I20" s="47"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="39"/>
-    </row>
-    <row r="21" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="38"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="22" t="s">
+      <c r="I21" s="45"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="37"/>
+    </row>
+    <row r="22" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="36"/>
+      <c r="G22" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="H21" s="20" t="s">
+      <c r="H22" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="I21" s="23" t="s">
+      <c r="I22" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="J21" s="31"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="39"/>
-    </row>
-    <row r="22" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="40"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="41"/>
-      <c r="M22" s="41"/>
-      <c r="N22" s="42"/>
-    </row>
-    <row r="23" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B24" s="26"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27"/>
-      <c r="N24" s="28"/>
-    </row>
+      <c r="N22" s="37"/>
+    </row>
+    <row r="23" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="38"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="40"/>
+    </row>
+    <row r="24" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B25" s="16"/>
-      <c r="C25" s="29" t="s">
+      <c r="B25" s="24"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="26"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B26" s="14"/>
+      <c r="C26" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="30" t="s">
+      <c r="D26" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E26" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="29"/>
-      <c r="K25" s="1" t="s">
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="18"/>
-    </row>
-    <row r="26" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="16"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="3" t="s">
+      <c r="L26" s="46"/>
+      <c r="M26" s="46"/>
+      <c r="N26" s="16"/>
+    </row>
+    <row r="27" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="14"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I26" s="29"/>
-      <c r="J26" s="29"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="18"/>
-    </row>
-    <row r="27" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="16"/>
-      <c r="C27" s="43" t="s">
+      <c r="I27" s="27"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="46"/>
+      <c r="L27" s="46"/>
+      <c r="M27" s="46"/>
+      <c r="N27" s="16"/>
+    </row>
+    <row r="28" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="14"/>
+      <c r="C28" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D28" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E27" s="44" t="s">
+      <c r="E28" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="F27" s="29"/>
-      <c r="G27" s="43" t="s">
+      <c r="F28" s="27"/>
+      <c r="G28" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="H27" s="7" t="s">
+      <c r="H28" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="44" t="s">
+      <c r="I28" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="J27" s="29"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="18"/>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B28" s="16"/>
-      <c r="C28" s="8" t="s">
+      <c r="J28" s="27"/>
+      <c r="K28" s="46"/>
+      <c r="L28" s="46"/>
+      <c r="M28" s="46"/>
+      <c r="N28" s="16"/>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B29" s="14"/>
+      <c r="C29" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D29" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E29" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F28" s="29"/>
-      <c r="G28" s="45" t="s">
+      <c r="F29" s="27"/>
+      <c r="G29" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="H28" s="46" t="s">
+      <c r="H29" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="I28" s="47"/>
-      <c r="J28" s="29"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="18"/>
-    </row>
-    <row r="29" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="16"/>
-      <c r="C29" s="13" t="s">
+      <c r="I29" s="45"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="46"/>
+      <c r="L29" s="46"/>
+      <c r="M29" s="46"/>
+      <c r="N29" s="16"/>
+    </row>
+    <row r="30" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="14"/>
+      <c r="C30" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D30" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E29" s="15"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="22" t="s">
+      <c r="E30" s="13"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="H29" s="20" t="s">
+      <c r="H30" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="I29" s="23" t="s">
+      <c r="I30" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="J29" s="29"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="18"/>
-    </row>
-    <row r="30" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="16"/>
-      <c r="C30" s="22" t="s">
+      <c r="J30" s="27"/>
+      <c r="K30" s="46"/>
+      <c r="L30" s="46"/>
+      <c r="M30" s="46"/>
+      <c r="N30" s="16"/>
+    </row>
+    <row r="31" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="14"/>
+      <c r="C31" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="20" t="s">
+      <c r="D31" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="E30" s="23" t="s">
+      <c r="E31" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="29"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="29"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="18"/>
-    </row>
-    <row r="31" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="32"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
-      <c r="K31" s="33"/>
-      <c r="L31" s="33"/>
-      <c r="M31" s="33"/>
-      <c r="N31" s="34"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="46"/>
+      <c r="M31" s="46"/>
+      <c r="N31" s="16"/>
     </row>
     <row r="32" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="24"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="24"/>
-      <c r="J32" s="24"/>
-      <c r="K32" s="24"/>
-      <c r="L32" s="24"/>
-      <c r="M32" s="24"/>
-      <c r="N32" s="24"/>
-    </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B33" s="26"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="27"/>
-      <c r="K33" s="27"/>
-      <c r="L33" s="27"/>
-      <c r="M33" s="27"/>
-      <c r="N33" s="28"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="31"/>
+      <c r="K32" s="31"/>
+      <c r="L32" s="31"/>
+      <c r="M32" s="31"/>
+      <c r="N32" s="32"/>
+    </row>
+    <row r="33" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="22"/>
+      <c r="M33" s="22"/>
+      <c r="N33" s="22"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B34" s="16"/>
-      <c r="C34" s="29" t="s">
+      <c r="B34" s="24"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="25"/>
+      <c r="L34" s="25"/>
+      <c r="M34" s="25"/>
+      <c r="N34" s="26"/>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B35" s="14"/>
+      <c r="C35" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="30" t="s">
+      <c r="D35" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="E34" s="31" t="s">
+      <c r="E35" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="F34" s="29"/>
-      <c r="G34" s="1" t="s">
+      <c r="F35" s="27"/>
+      <c r="G35" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="18"/>
-    </row>
-    <row r="35" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="16"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="18"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="46"/>
+      <c r="J35" s="46"/>
+      <c r="K35" s="46"/>
+      <c r="L35" s="46"/>
+      <c r="M35" s="46"/>
+      <c r="N35" s="16"/>
     </row>
     <row r="36" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="16"/>
-      <c r="C36" s="43" t="s">
+      <c r="B36" s="14"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="46"/>
+      <c r="H36" s="46"/>
+      <c r="I36" s="46"/>
+      <c r="J36" s="46"/>
+      <c r="K36" s="46"/>
+      <c r="L36" s="46"/>
+      <c r="M36" s="46"/>
+      <c r="N36" s="16"/>
+    </row>
+    <row r="37" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="14"/>
+      <c r="C37" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D37" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E36" s="44" t="s">
+      <c r="E37" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="F36" s="29"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-      <c r="N36" s="18"/>
-    </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B37" s="16"/>
-      <c r="C37" s="8" t="s">
+      <c r="F37" s="27"/>
+      <c r="G37" s="46"/>
+      <c r="H37" s="46"/>
+      <c r="I37" s="46"/>
+      <c r="J37" s="46"/>
+      <c r="K37" s="46"/>
+      <c r="L37" s="46"/>
+      <c r="M37" s="46"/>
+      <c r="N37" s="16"/>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B38" s="14"/>
+      <c r="C38" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D38" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E38" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F37" s="29"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="18"/>
-    </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B38" s="16"/>
-      <c r="C38" s="13" t="s">
+      <c r="F38" s="27"/>
+      <c r="G38" s="46"/>
+      <c r="H38" s="46"/>
+      <c r="I38" s="46"/>
+      <c r="J38" s="46"/>
+      <c r="K38" s="46"/>
+      <c r="L38" s="46"/>
+      <c r="M38" s="46"/>
+      <c r="N38" s="16"/>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B39" s="14"/>
+      <c r="C39" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="D39" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E38" s="15" t="s">
+      <c r="E39" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="F38" s="29"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-      <c r="N38" s="18"/>
-    </row>
-    <row r="39" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="16"/>
-      <c r="C39" s="22" t="s">
+      <c r="F39" s="27"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="46"/>
+      <c r="I39" s="46"/>
+      <c r="J39" s="46"/>
+      <c r="K39" s="46"/>
+      <c r="L39" s="46"/>
+      <c r="M39" s="46"/>
+      <c r="N39" s="16"/>
+    </row>
+    <row r="40" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="14"/>
+      <c r="C40" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="D39" s="20" t="s">
+      <c r="D40" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="E39" s="23" t="s">
+      <c r="E40" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F39" s="29"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
-      <c r="N39" s="18"/>
-    </row>
-    <row r="40" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="32"/>
-      <c r="C40" s="33"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="33"/>
-      <c r="H40" s="33"/>
-      <c r="I40" s="33"/>
-      <c r="J40" s="33"/>
-      <c r="K40" s="33"/>
-      <c r="L40" s="33"/>
-      <c r="M40" s="33"/>
-      <c r="N40" s="34"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="46"/>
+      <c r="H40" s="46"/>
+      <c r="I40" s="46"/>
+      <c r="J40" s="46"/>
+      <c r="K40" s="46"/>
+      <c r="L40" s="46"/>
+      <c r="M40" s="46"/>
+      <c r="N40" s="16"/>
+    </row>
+    <row r="41" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="30"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
+      <c r="H41" s="31"/>
+      <c r="I41" s="31"/>
+      <c r="J41" s="31"/>
+      <c r="K41" s="31"/>
+      <c r="L41" s="31"/>
+      <c r="M41" s="31"/>
+      <c r="N41" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="G34:M39"/>
-    <mergeCell ref="K25:M30"/>
+    <mergeCell ref="G35:M40"/>
+    <mergeCell ref="K26:M31"/>
     <mergeCell ref="K17:M21"/>
     <mergeCell ref="G13:M13"/>
   </mergeCells>

</xml_diff>

<commit_message>
added 'rx buffer available' flag in RXPacket
</commit_message>
<xml_diff>
--- a/Protocol.xlsx
+++ b/Protocol.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="62">
   <si>
     <t>Description</t>
   </si>
@@ -200,7 +200,16 @@
     <t>flush buffers, reset configuration. no data payload</t>
   </si>
   <si>
-    <t>Last TX Acknowledged</t>
+    <t>Pipe, Status</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>RX Buffer Available</t>
+  </si>
+  <si>
+    <t>See 'Pipe, Status'</t>
   </si>
 </sst>
 </file>
@@ -649,7 +658,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -791,6 +800,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1106,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q41"/>
+  <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1582,32 +1597,34 @@
         <v>44</v>
       </c>
       <c r="F20" s="29"/>
-      <c r="G20" s="9">
-        <v>7</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="I20" s="10"/>
+      <c r="G20" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="I20" s="45"/>
       <c r="J20" s="29"/>
       <c r="K20" s="47"/>
       <c r="L20" s="47"/>
       <c r="M20" s="47"/>
       <c r="N20" s="37"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="36"/>
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
       <c r="E21" s="29"/>
       <c r="F21" s="29"/>
-      <c r="G21" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="H21" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="I21" s="45"/>
+      <c r="G21" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I21" s="21" t="s">
+        <v>40</v>
+      </c>
       <c r="J21" s="29"/>
       <c r="K21" s="47"/>
       <c r="L21" s="47"/>
@@ -1615,135 +1632,147 @@
       <c r="N21" s="37"/>
     </row>
     <row r="22" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="36"/>
-      <c r="G22" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="H22" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="I22" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="N22" s="37"/>
-    </row>
-    <row r="23" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="38"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="39"/>
-      <c r="M23" s="39"/>
-      <c r="N23" s="40"/>
-    </row>
-    <row r="24" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B25" s="24"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="25"/>
-      <c r="N25" s="26"/>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B22" s="38"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="39"/>
+      <c r="N22" s="40"/>
+    </row>
+    <row r="23" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B24" s="24"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="26"/>
+    </row>
+    <row r="25" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="14"/>
+      <c r="C25" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="L25" s="46"/>
+      <c r="M25" s="46"/>
+      <c r="N25" s="16"/>
+    </row>
+    <row r="26" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="14"/>
-      <c r="C26" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26" s="29" t="s">
-        <v>53</v>
-      </c>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
       <c r="F26" s="27"/>
       <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
+      <c r="H26" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="I26" s="27"/>
       <c r="J26" s="27"/>
-      <c r="K26" s="46" t="s">
-        <v>56</v>
-      </c>
+      <c r="K26" s="46"/>
       <c r="L26" s="46"/>
       <c r="M26" s="46"/>
       <c r="N26" s="16"/>
     </row>
     <row r="27" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="14"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
+      <c r="C27" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="42" t="s">
+        <v>6</v>
+      </c>
       <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I27" s="27"/>
+      <c r="G27" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I27" s="42" t="s">
+        <v>6</v>
+      </c>
       <c r="J27" s="27"/>
       <c r="K27" s="46"/>
       <c r="L27" s="46"/>
       <c r="M27" s="46"/>
       <c r="N27" s="16"/>
     </row>
-    <row r="28" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" s="14"/>
-      <c r="C28" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E28" s="42" t="s">
-        <v>6</v>
+      <c r="C28" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="F28" s="27"/>
-      <c r="G28" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="I28" s="42" t="s">
-        <v>6</v>
-      </c>
+      <c r="G28" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="H28" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="I28" s="45"/>
       <c r="J28" s="27"/>
       <c r="K28" s="46"/>
       <c r="L28" s="46"/>
       <c r="M28" s="46"/>
       <c r="N28" s="16"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="14"/>
-      <c r="C29" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>29</v>
-      </c>
+      <c r="C29" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" s="13"/>
       <c r="F29" s="27"/>
-      <c r="G29" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="H29" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="I29" s="45"/>
+      <c r="G29" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="H29" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I29" s="21" t="s">
+        <v>40</v>
+      </c>
       <c r="J29" s="27"/>
       <c r="K29" s="46"/>
       <c r="L29" s="46"/>
@@ -1752,23 +1781,19 @@
     </row>
     <row r="30" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="14"/>
-      <c r="C30" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E30" s="13"/>
+      <c r="C30" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>37</v>
+      </c>
       <c r="F30" s="27"/>
-      <c r="G30" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="H30" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="I30" s="21" t="s">
-        <v>40</v>
-      </c>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
       <c r="J30" s="27"/>
       <c r="K30" s="46"/>
       <c r="L30" s="46"/>
@@ -1776,89 +1801,85 @@
       <c r="N30" s="16"/>
     </row>
     <row r="31" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="14"/>
-      <c r="C31" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D31" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="E31" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
-      <c r="K31" s="46"/>
-      <c r="L31" s="46"/>
-      <c r="M31" s="46"/>
-      <c r="N31" s="16"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="31"/>
+      <c r="K31" s="31"/>
+      <c r="L31" s="31"/>
+      <c r="M31" s="31"/>
+      <c r="N31" s="32"/>
     </row>
     <row r="32" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="30"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="31"/>
-      <c r="K32" s="31"/>
-      <c r="L32" s="31"/>
-      <c r="M32" s="31"/>
-      <c r="N32" s="32"/>
-    </row>
-    <row r="33" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="22"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="22"/>
-      <c r="K33" s="22"/>
-      <c r="L33" s="22"/>
-      <c r="M33" s="22"/>
-      <c r="N33" s="22"/>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B34" s="24"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="25"/>
-      <c r="L34" s="25"/>
-      <c r="M34" s="25"/>
-      <c r="N34" s="26"/>
-    </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
+      <c r="L32" s="22"/>
+      <c r="M32" s="22"/>
+      <c r="N32" s="22"/>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B33" s="24"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="25"/>
+      <c r="L33" s="25"/>
+      <c r="M33" s="25"/>
+      <c r="N33" s="26"/>
+    </row>
+    <row r="34" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="14"/>
+      <c r="C34" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="F34" s="27"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="48"/>
+      <c r="I34" s="48"/>
+      <c r="J34" s="48"/>
+      <c r="K34" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="L34" s="46"/>
+      <c r="M34" s="46"/>
+      <c r="N34" s="16"/>
+    </row>
+    <row r="35" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="14"/>
-      <c r="C35" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="D35" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="E35" s="29" t="s">
-        <v>54</v>
-      </c>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
       <c r="F35" s="27"/>
-      <c r="G35" s="46" t="s">
-        <v>46</v>
-      </c>
-      <c r="H35" s="46"/>
-      <c r="I35" s="46"/>
-      <c r="J35" s="46"/>
+      <c r="G35" s="48"/>
+      <c r="H35" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="I35" s="48"/>
+      <c r="J35" s="48"/>
       <c r="K35" s="46"/>
       <c r="L35" s="46"/>
       <c r="M35" s="46"/>
@@ -1866,124 +1887,125 @@
     </row>
     <row r="36" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="14"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
+      <c r="C36" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E36" s="42" t="s">
+        <v>6</v>
+      </c>
       <c r="F36" s="27"/>
-      <c r="G36" s="46"/>
-      <c r="H36" s="46"/>
-      <c r="I36" s="46"/>
-      <c r="J36" s="46"/>
+      <c r="G36" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I36" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="J36" s="48"/>
       <c r="K36" s="46"/>
       <c r="L36" s="46"/>
       <c r="M36" s="46"/>
       <c r="N36" s="16"/>
     </row>
-    <row r="37" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B37" s="14"/>
-      <c r="C37" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E37" s="42" t="s">
-        <v>6</v>
+      <c r="C37" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="F37" s="27"/>
-      <c r="G37" s="46"/>
-      <c r="H37" s="46"/>
-      <c r="I37" s="46"/>
-      <c r="J37" s="46"/>
+      <c r="G37" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="H37" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="I37" s="45"/>
+      <c r="J37" s="48"/>
       <c r="K37" s="46"/>
       <c r="L37" s="46"/>
       <c r="M37" s="46"/>
       <c r="N37" s="16"/>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="14"/>
-      <c r="C38" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D38" s="7" t="s">
+      <c r="C38" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F38" s="27"/>
+      <c r="G38" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="I38" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F38" s="27"/>
-      <c r="G38" s="46"/>
-      <c r="H38" s="46"/>
-      <c r="I38" s="46"/>
-      <c r="J38" s="46"/>
+      <c r="J38" s="48"/>
       <c r="K38" s="46"/>
       <c r="L38" s="46"/>
       <c r="M38" s="46"/>
       <c r="N38" s="16"/>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" s="14"/>
-      <c r="C39" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>40</v>
+      <c r="C39" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E39" s="21" t="s">
+        <v>42</v>
       </c>
       <c r="F39" s="27"/>
-      <c r="G39" s="46"/>
-      <c r="H39" s="46"/>
-      <c r="I39" s="46"/>
-      <c r="J39" s="46"/>
+      <c r="G39" s="48"/>
+      <c r="H39" s="48"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="48"/>
       <c r="K39" s="46"/>
       <c r="L39" s="46"/>
       <c r="M39" s="46"/>
       <c r="N39" s="16"/>
     </row>
     <row r="40" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="14"/>
-      <c r="C40" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D40" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="E40" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="F40" s="27"/>
-      <c r="G40" s="46"/>
-      <c r="H40" s="46"/>
-      <c r="I40" s="46"/>
-      <c r="J40" s="46"/>
-      <c r="K40" s="46"/>
-      <c r="L40" s="46"/>
-      <c r="M40" s="46"/>
-      <c r="N40" s="16"/>
-    </row>
-    <row r="41" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="30"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="31"/>
-      <c r="H41" s="31"/>
-      <c r="I41" s="31"/>
-      <c r="J41" s="31"/>
-      <c r="K41" s="31"/>
-      <c r="L41" s="31"/>
-      <c r="M41" s="31"/>
-      <c r="N41" s="32"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="31"/>
+      <c r="H40" s="31"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
+      <c r="K40" s="31"/>
+      <c r="L40" s="31"/>
+      <c r="M40" s="31"/>
+      <c r="N40" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="G35:M40"/>
-    <mergeCell ref="K26:M31"/>
     <mergeCell ref="K17:M21"/>
     <mergeCell ref="G13:M13"/>
+    <mergeCell ref="K25:M30"/>
+    <mergeCell ref="K34:M39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>